<commit_message>
update charging resistor on tritag
</commit_message>
<xml_diff>
--- a/pcb/tritag/rev_b/tritag_bom.xlsx
+++ b/pcb/tritag/rev_b/tritag_bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="125">
   <si>
     <t>Qty</t>
   </si>
@@ -278,13 +278,10 @@
     <t>RHM1.0KCECT-ND</t>
   </si>
   <si>
-    <t>2k 1%</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>RHM2KCDCT-ND</t>
+    <t>RHM560CDCT-ND</t>
   </si>
   <si>
     <t>10k</t>
@@ -481,7 +478,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -496,6 +493,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -529,7 +530,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1008,8 +1009,8 @@
       <c r="A20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>87</v>
+      <c r="B20" s="4" t="n">
+        <v>560</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>82</v>
@@ -1018,13 +1019,13 @@
         <v>83</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>85</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>82</v>
@@ -1041,13 +1042,13 @@
         <v>83</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>85</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,7 +1056,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>82</v>
@@ -1064,13 +1065,13 @@
         <v>83</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>85</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>82</v>
@@ -1087,13 +1088,13 @@
         <v>83</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>85</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>82</v>
@@ -1110,13 +1111,13 @@
         <v>83</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>85</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,25 +1125,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="G25" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="H25" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,19 +1151,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="F26" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,22 +1171,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="E27" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="F27" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="G27" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,22 +1194,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="0" t="s">
+      <c r="E28" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="F28" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="G28" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,22 +1217,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>